<commit_message>
ajustes y exportar imgs de pantallas
</commit_message>
<xml_diff>
--- a/MasPruebas/excel/caso02_sanoperioexito.xlsx
+++ b/MasPruebas/excel/caso02_sanoperioexito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uxi\Documents\TFG\MasPruebas\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D733B9B-F53C-4300-A559-9AA9B2C67032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84E31C6-A699-40A5-B4CC-A1CBE0AE95AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,11 +574,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CG14"/>
   <sheetViews>
-    <sheetView topLeftCell="BM1" workbookViewId="0">
-      <selection activeCell="CH14" sqref="CH14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:85" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
@@ -3568,8 +3571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>